<commit_message>
added MFCC to heatmap, removed clustermap
</commit_message>
<xml_diff>
--- a/data/inputs/speech_psychiatry_figure2.xlsx
+++ b/data/inputs/speech_psychiatry_figure2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>Possible values between -1 (lower than controls) and 1 (higher than controls). We add up papers: conflicting findings. Non-significant = 0 if no positive finding, but x*0.5 if other findings to reduce effect.
 Format: "value, Author et al. (year)" for one article or "value, Author et al. (year); value, Author et al. (year)" for more than one article. Add first word of title if multiple articles per author, eg: "value, Author et al. (year) FirstWord"</t>
@@ -77,7 +77,7 @@
     <t>HNR</t>
   </si>
   <si>
-    <t>0, Horwitz et al. (2013); 0, Horwitz et al. (2013); 0, Vicsi et al. (2012)</t>
+    <t>0, Horwitz et al. (2013); 0, Horwitz et al. (2013); 0, Vicsi et al. (2012); 1, Quatieri and Malyska (2012); 1, Quatieri and Malyska (2012)</t>
   </si>
   <si>
     <t>0, Ferreira et al. (2010)</t>
@@ -173,6 +173,18 @@
     <t>1, (Zhang et al. 2018); 1, Zhang et al. (2018)</t>
   </si>
   <si>
+    <t>MFCC</t>
+  </si>
+  <si>
+    <t>-1, Cummins et al. (2013); -1, Cummins et al. (2015); -1, Cummins et al. (2015)</t>
+  </si>
+  <si>
+    <t>-1, Zhang et al. (2016); 1, Wörtwein (2017)</t>
+  </si>
+  <si>
+    <t>-1, Zhang et al. (2018)</t>
+  </si>
+  <si>
     <t>prosody</t>
   </si>
   <si>
@@ -233,16 +245,13 @@
     <t>Intensity variability</t>
   </si>
   <si>
-    <t>-1, Quatieri and Malyska (2012); -1, Alghowinem et al. (2013) Chacterising</t>
+    <t>-1, Quatieri and Malyska (2012); -1, Alghowinem et al. (2013) Chacterising; -1, Quatieri and Malyska (2012); -1, Cummins et al. (2013); -1, Cummins et al. (2015); 1, Cummins et al. (2015); -1, Horwitz et al. (2013); -1, Horwitz et al. (2013); 0, Horwitz et al. (2013); -1, Horwitz et al. (2013)</t>
   </si>
   <si>
     <t>1, Rapcan. et al. (2010); 1, Rapcan et al. (2010); 0, Martínez-Sánchez et al. (2015); 1, Kliper. et al. (2015); 0, Kliper. et al. (2015); 0, Kliper. et al. (2015); 0, Meaux et al. (2018); 0, Meaux et al. (2018); -1, Kliper et al. (2010); 0, Bedwell et al. (2014); 0, Bedwell et al. (2014)</t>
   </si>
   <si>
     <t>Energy variance</t>
-  </si>
-  <si>
-    <t>-1, Quatieri and Malyska (2012); -1, Cummins et al. (2013); -1, Cummins et al. (2015); 1, Cummins et al. (2015); -1, Horwitz et al. (2013); -1, Horwitz et al. (2013); 0, Horwitz et al. (2013); -1, Horwitz et al. (2013)</t>
   </si>
   <si>
     <t>Energy velocity</t>
@@ -257,7 +266,7 @@
     <t>Speech rate</t>
   </si>
   <si>
-    <t>-1, Mundt et al. (2012); -1, Alghowinem et al. (2012); -1, Hönig et al. (2014)</t>
+    <t>-1, Mundt et al. (2012); -1, Alghowinem et al. (2012); -1, Hönig et al. (2014); -1, Trevino et al. (2011)</t>
   </si>
   <si>
     <t>-1, Perlini et al. (2012); 0, Docherty et al. (2012); -1, Tahir et al. (2019)</t>
@@ -269,7 +278,7 @@
     <t>Articulation rate</t>
   </si>
   <si>
-    <t>0, Scherer et al. (2013); -1, Kiss et al. (2017); -1, Kiss et al. (2017)</t>
+    <t>0, Scherer et al. (2013); -1, Kiss et al. (2017); -1, Kiss et al. (2017); 0, Wolters et al. (2015)</t>
   </si>
   <si>
     <t xml:space="preserve">Time talking </t>
@@ -287,7 +296,7 @@
     <t>Pause duration mean</t>
   </si>
   <si>
-    <t>0, Yang et al. (2012); -1, Alghowinem et al. (2012)</t>
+    <t>0, Yang et al. (2012); -1, Alghowinem et al. (2012); 0, Wolters et al. (2015); 1, Trevino et al. (2011)</t>
   </si>
   <si>
     <t>0, Martínez-Sánchez et al. (2015); 1, Kliper. et al. (2015); 0, Rapcan et al. (2010); 1, Rapcan et al. (2010); 1, Kliper et al. (2010)</t>
@@ -305,7 +314,7 @@
     <t>Pause rate</t>
   </si>
   <si>
-    <t>-1, Alghowinem et al. (2012); -1, Kiss et al. (2017); -1, Kiss et al. (2017)</t>
+    <t>-1, Alghowinem et al. (2012); -1, Kiss et al. (2017); -1, Kiss et al. (2017); -1, Trevino et al. (2011)</t>
   </si>
   <si>
     <t>-1, Martínez-Sánchez et al. (2015)</t>
@@ -314,7 +323,7 @@
     <t>Pauses total</t>
   </si>
   <si>
-    <t>1, Guidi et al. (2017); 0, Guidi et al. (2017); 1, Martinez-Sanchez et al. (2015)</t>
+    <t>1, Guidi et al. (2017); 0, Guidi et al. (2017); 1, Martinez-Sanchez et al. (2015); 0, Wolters et al. (2015)</t>
   </si>
   <si>
     <t>1, Rapcan. et al. (2010); 0, Rapcan et al. (2010); -1, Matsumoto et al. (2013); 1, Dickey et al. (2012); 0, Bedwell et al. (2014); 0, Bedwell et al. (2014)</t>
@@ -327,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -355,6 +364,13 @@
       <sz val="8.0"/>
       <color rgb="FFFF0000"/>
     </font>
+    <font>
+      <sz val="8.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -376,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -409,6 +425,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
@@ -1300,31 +1325,25 @@
       <c r="AM18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="I19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>59</v>
+      <c r="J19" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1357,25 +1376,31 @@
       <c r="AM19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1408,24 +1433,26 @@
       <c r="AM20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="2" t="s">
         <v>67</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="J21" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
@@ -1457,24 +1484,24 @@
       <c r="AM21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="4"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -1510,7 +1537,7 @@
       <c r="B23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D23" s="4"/>
@@ -1521,7 +1548,9 @@
         <v>74</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1553,20 +1582,22 @@
       <c r="AM23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="9"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>76</v>
+      <c r="C24" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="2"/>
+      <c r="J24" s="4"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1600,15 +1631,13 @@
     <row r="25">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="C25" s="3"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="4"/>
       <c r="H25" s="2"/>
       <c r="I25" s="4"/>
       <c r="J25" s="2"/>
@@ -1644,16 +1673,16 @@
     </row>
     <row r="26">
       <c r="A26" s="9"/>
-      <c r="B26" s="9" t="s">
-        <v>79</v>
+      <c r="B26" s="2" t="s">
+        <v>80</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="4"/>
       <c r="J26" s="2"/>
@@ -1689,23 +1718,19 @@
     </row>
     <row r="27">
       <c r="A27" s="9"/>
-      <c r="B27" s="2" t="s">
-        <v>80</v>
+      <c r="B27" s="9" t="s">
+        <v>82</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="2" t="s">
-        <v>82</v>
+      <c r="G27" s="2" t="s">
+        <v>70</v>
       </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -1737,24 +1762,24 @@
       <c r="AM27" s="5"/>
     </row>
     <row r="28">
-      <c r="A28" s="4"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="3" t="s">
-        <v>27</v>
+      <c r="H28" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -1787,16 +1812,20 @@
     </row>
     <row r="29">
       <c r="A29" s="4"/>
-      <c r="B29" s="2" t="s">
-        <v>86</v>
+      <c r="B29" s="9" t="s">
+        <v>87</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="3" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1833,15 +1862,15 @@
     <row r="30">
       <c r="A30" s="4"/>
       <c r="B30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="2" t="s">
-        <v>89</v>
+      <c r="H30" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -1878,21 +1907,17 @@
     <row r="31">
       <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -1927,17 +1952,21 @@
     <row r="32">
       <c r="A32" s="4"/>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="H32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -1972,20 +2001,18 @@
     <row r="33">
       <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="2"/>
+      <c r="J33" s="4"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
@@ -2021,20 +2048,18 @@
       <c r="B34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
@@ -2067,6 +2092,29 @@
     </row>
     <row r="35">
       <c r="A35" s="4"/>
+      <c r="B35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
@@ -2092,22 +2140,7 @@
       <c r="AM35" s="5"/>
     </row>
     <row r="36">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
+      <c r="A36" s="4"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
@@ -2135,7 +2168,7 @@
     <row r="37">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="11"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2176,7 +2209,7 @@
     <row r="38">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="11"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -2217,7 +2250,7 @@
     <row r="39">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2585,7 +2618,7 @@
     </row>
     <row r="48">
       <c r="A48" s="5"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -2626,7 +2659,7 @@
     </row>
     <row r="49">
       <c r="A49" s="5"/>
-      <c r="B49" s="11"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -2667,7 +2700,7 @@
     </row>
     <row r="50">
       <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -41943,6 +41976,47 @@
       <c r="AL1007" s="5"/>
       <c r="AM1007" s="5"/>
     </row>
+    <row r="1008">
+      <c r="A1008" s="5"/>
+      <c r="B1008" s="5"/>
+      <c r="C1008" s="5"/>
+      <c r="D1008" s="5"/>
+      <c r="E1008" s="5"/>
+      <c r="F1008" s="5"/>
+      <c r="G1008" s="5"/>
+      <c r="H1008" s="5"/>
+      <c r="I1008" s="5"/>
+      <c r="J1008" s="5"/>
+      <c r="K1008" s="5"/>
+      <c r="L1008" s="5"/>
+      <c r="M1008" s="5"/>
+      <c r="N1008" s="5"/>
+      <c r="O1008" s="5"/>
+      <c r="P1008" s="5"/>
+      <c r="Q1008" s="5"/>
+      <c r="R1008" s="5"/>
+      <c r="S1008" s="5"/>
+      <c r="T1008" s="5"/>
+      <c r="U1008" s="5"/>
+      <c r="V1008" s="5"/>
+      <c r="W1008" s="5"/>
+      <c r="X1008" s="5"/>
+      <c r="Y1008" s="5"/>
+      <c r="Z1008" s="5"/>
+      <c r="AA1008" s="5"/>
+      <c r="AB1008" s="5"/>
+      <c r="AC1008" s="5"/>
+      <c r="AD1008" s="5"/>
+      <c r="AE1008" s="5"/>
+      <c r="AF1008" s="5"/>
+      <c r="AG1008" s="5"/>
+      <c r="AH1008" s="5"/>
+      <c r="AI1008" s="5"/>
+      <c r="AJ1008" s="5"/>
+      <c r="AK1008" s="5"/>
+      <c r="AL1008" s="5"/>
+      <c r="AM1008" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>

</xml_diff>